<commit_message>
Module 7 Advanced Movie Search
This Process:

1. Search a movie based on the user input in the movie search (https://rpachallenge.com/movieSearch)

2. Respective the name and description.

3. Write the description to notepad.

4. Save the notepad with the movie name.
</commit_message>
<xml_diff>
--- a/RPA018_UiAutomationWithTheModernExperience_04_TableExtraction/UiPath Academy.xlsx
+++ b/RPA018_UiAutomationWithTheModernExperience_04_TableExtraction/UiPath Academy.xlsx
@@ -14,123 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
-  <x:si>
-    <x:t>RPA Video Tutorials - UiPath</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.uipath.com/learning/video-tutorials</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy - The School for the Future of Work - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=qt3vPjeoloc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Story of Work: UiPath Academy - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=5Vubyka_-lY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy 2 - advanced RPA learning program - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=A3Ccghq8bIQ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy - A Year in Review (2018) - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=kDZ1VEAHX6U</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy 2-Year Anniversary - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=DTX_wdydipM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy Live Paris - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=KPN7zIkP05k</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy Live - mastering the RPA essentials - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=7rjVCNYVd_Q</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy Live: Mastering the RPA Essentials - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=GEcAp8cx0CU</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RPA UiPath Tutorial For Beginners | RPA Course - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=kg15yZiBGxE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Workflow Automation Tutorial - UiPath Studio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.uipath.com/learning/video-tutorials/workflow-automation-uipath-studio</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy #shorts - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=_COLHLsEBQI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy - One year of Love for Automation - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=EHIRiooQ5c0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RegEx || UiPath Academy || RPA Developer Foundation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=KtLtQYHIOa0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LIVE Conversation | UiPath Academy - YouTube - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=Xu_U3xiAyEg</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="247">
+  <x:si>
+    <x:t>Video Demo - Working with Lists || UiPath Academy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=a9xmh7q4oy8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 abr 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nisarg Kadam | Day 1 - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=wS_tBYSYKpQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 oct 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reskilling with UiPath Academy: Jay Armand Ogayon - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=Wk5-aCLVIoA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17 jul 2020</x:t>
   </x:si>
   <x:si>
     <x:t>UiPath Academy || RPA Developer Foundation - YouTube</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.youtube.com/watch?v=ZUIRWWadT4A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath on X: "Cheers to 5 years of UiPath Academy! Here's to ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://twitter.com/UiPath/status/1540364198147915776</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=cuYeT7dOu94</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unlock New Opportunities with UiPath Certification - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=__gkKr6LWQA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Video Demo - Working with Lists || UiPath Academy - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=a9xmh7q4oy8</x:t>
+    <x:t>https://www.youtube.com/watch?v=UVN_pScqF1c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OCR methods || UiPath Academy || RPA Developer Foundation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=1IP8dpMuuP0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30 abr 2020</x:t>
   </x:si>
   <x:si>
     <x:t>Extract as Workflow, Invoke Workflow &amp; Arguments - YouTube</x:t>
@@ -139,73 +67,145 @@
     <x:t>https://www.youtube.com/watch?v=yLeV_PCa74k</x:t>
   </x:si>
   <x:si>
-    <x:t>Quiz 8: Email Automation || UiPath Academy || RPA Developer ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=RoUb_cjSUOA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stay in the Loop: Exciting Updates from UiPath Insider Portal ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=lSSv7qUqReA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy Live training - London. Learn RPA. | Facebook</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.facebook.com/UiPath/videos/uipath-academy-live-training-london-learn-rpa/591121434645598/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Reskilling with UiPath Academy: Jay Armand Ogayon - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=Wk5-aCLVIoA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=UVN_pScqF1c</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OCR methods || UiPath Academy || RPA Developer Foundation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=1IP8dpMuuP0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nisarg Kadam | Day 1 - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=wS_tBYSYKpQ</x:t>
+    <x:t>5 may 2020</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=UiofV2T4Dto</x:t>
   </x:si>
   <x:si>
+    <x:t>8 abr 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>Quiz 1: Variables,Data Types and Control Flow || UiPath ...</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=ztArcqLmevw</x:t>
   </x:si>
   <x:si>
+    <x:t>26 abr 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.youtube.com/watch?v=JjQMIspg5FU</x:t>
   </x:si>
   <x:si>
+    <x:t>How to choose UiPath RPA Certification for your ... - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=0G7bKbrrpEQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11 abr 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Test Suite || TheRPAGuy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=GKOsykcec10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 mar 2021</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.youtube.com/watch?v=x-mlbaBcn8Y</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.youtube.com/watch?v=HYKb2AOG3WE</x:t>
-  </x:si>
-  <x:si>
     <x:t>Test Activity and Create Test Bench || UiPath Academy</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=dkbYI15Yqe8</x:t>
   </x:si>
   <x:si>
-    <x:t>UiPath Test Suite || TheRPAGuy - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=GKOsykcec10</x:t>
+    <x:t>6 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Academy || Building Data Driven Test Cases with ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=lJdWgrC77Dc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Scraping || UiPath Academy || RPA Developer Foundation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=I_s9jrBWZr8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Video Demo - Screen scraping || UiPath Academy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=srBM3dGNuV4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Academy || RPA Developer Foundation - Debugging</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=2OWncRRGYeQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quiz 10: Robotic Enterprise Framework Overview ... - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=rm0x3CA4css</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UI Interactions || UiPath Academy || RPA Developer Foundation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=EzdHCjTQVt4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA Developer Foundation - Quiz 11: PDF Automation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=u_O2AT4Bees</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Watch Panel - RPA Developer Foundation - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=_wphrAQrkn8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Parte3] Assignment 1: Calculate Client Security Hash</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=TlnMXuySL9M</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Video Demo - Managing Difficult Situations || UiPath Academy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=jt0ytItsMSI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Introduction to Selectors || UiPath Academy - Video Demo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=IckbAodbV_o</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Anchor Base Activity || UiPath Academy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=-A9uPRy22xc</x:t>
   </x:si>
   <x:si>
     <x:t>[Parte2] Assignment 1: Calculate Client Security Hash</x:t>
@@ -214,88 +214,7 @@
     <x:t>https://www.youtube.com/watch?v=fx264neyD7U</x:t>
   </x:si>
   <x:si>
-    <x:t>UiPath Academy || Building Data Driven Test Cases with ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=lJdWgrC77Dc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Data Scraping || UiPath Academy || RPA Developer Foundation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=I_s9jrBWZr8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>How to choose UiPath RPA Certification for your ... - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=0G7bKbrrpEQ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Video Demo - Screen scraping || UiPath Academy - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=srBM3dGNuV4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy Overview | This year we've embarked into an ...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.facebook.com/UiPath/videos/uipath-academy-overview/2274898056118825/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UiPath Academy || RPA Developer Foundation - Debugging</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=2OWncRRGYeQ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Quiz 10: Robotic Enterprise Framework Overview ... - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=rm0x3CA4css</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UI Interactions || UiPath Academy || RPA Developer Foundation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=EzdHCjTQVt4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RPA Developer Foundation - Quiz 11: PDF Automation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=u_O2AT4Bees</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Watch Panel - RPA Developer Foundation - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=_wphrAQrkn8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[Parte3] Assignment 1: Calculate Client Security Hash</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=TlnMXuySL9M</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Video Demo - Managing Difficult Situations || UiPath Academy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=jt0ytItsMSI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Introduction to Selectors || UiPath Academy - Video Demo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=IckbAodbV_o</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Anchor Base Activity || UiPath Academy - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=-A9uPRy22xc</x:t>
+    <x:t>28 may 2020</x:t>
   </x:si>
   <x:si>
     <x:t>Quiz 9: Orchestrator for Developers || UiPath Academy</x:t>
@@ -316,10 +235,10 @@
     <x:t>https://www.youtube.com/watch?v=Z_N2P9GYblo</x:t>
   </x:si>
   <x:si>
-    <x:t>UiPath Academy ビデオチュートリアル - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/playlist?list=PLQBe36ilIwgio4a2QA237px8ToUmdGj12</x:t>
+    <x:t>Video Demo - Retry Scope || UiPath Academy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=huQx4TlUgUM</x:t>
   </x:si>
   <x:si>
     <x:t>UiPath Test Manager in Action - YouTube</x:t>
@@ -328,61 +247,82 @@
     <x:t>https://www.youtube.com/watch?v=tvabMvYPymQ</x:t>
   </x:si>
   <x:si>
-    <x:t>Video Demo - Retry Scope || UiPath Academy - YouTube</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=huQx4TlUgUM</x:t>
-  </x:si>
-  <x:si>
     <x:t>UiPath Academy Hash Assignment - YouTube</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=JqR926wSwck</x:t>
   </x:si>
   <x:si>
+    <x:t>17 abr 2018</x:t>
+  </x:si>
+  <x:si>
     <x:t>Create your first workflow in UiPath Studio - YouTube</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=xDyvR9G0IYI</x:t>
   </x:si>
   <x:si>
+    <x:t>9 abr 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>Video Demo - Working with Excel files 1 || UiPath Academy</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=EoM0qZlojcM</x:t>
   </x:si>
   <x:si>
+    <x:t>27 abr 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>Extracting Data from PDF || UiPath Academy - YouTube</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=PucDkxbQU84</x:t>
   </x:si>
   <x:si>
+    <x:t>Video Demo - Working with UI elements || UiPath Academy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=ucFVNHOCzYY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29 abr 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>Using Index Variables in Selectors || UiPath Academy || RPA ...</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=hCvx2vwdnGI</x:t>
   </x:si>
   <x:si>
+    <x:t>2 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>State Machine || UiPath Academy || RPA Developer Foundation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=-rXkMkZXLR4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=N9bGajGpaU8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22 abr 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Using Property Explorer || UiPath Academy - Video Demo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=79HX9e-imtA</x:t>
+  </x:si>
+  <x:si>
     <x:t>UiPath Academy free Online Diploma Courses with Certificate</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=0n7Myuh5kho</x:t>
   </x:si>
   <x:si>
-    <x:t>State Machine || UiPath Academy || RPA Developer Foundation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=-rXkMkZXLR4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=N9bGajGpaU8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Using Property Explorer || UiPath Academy - Video Demo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=79HX9e-imtA</x:t>
+    <x:t>4 jul 2020</x:t>
   </x:si>
   <x:si>
     <x:t>[Parte4] Assignment 1: Calculate Client Security Hash</x:t>
@@ -391,9 +331,15 @@
     <x:t>https://www.youtube.com/watch?v=lk7cYC8WHSA</x:t>
   </x:si>
   <x:si>
+    <x:t>30 may 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.youtube.com/watch?v=-EurQb2Y-V8</x:t>
   </x:si>
   <x:si>
+    <x:t>10 abr 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>The Immediate Panel - RPA Developer Foundationl - YouTube</x:t>
   </x:si>
   <x:si>
@@ -418,28 +364,28 @@
     <x:t>https://www.youtube.com/watch?v=ZmmUebaXEwI</x:t>
   </x:si>
   <x:si>
+    <x:t>21 jun 2019</x:t>
+  </x:si>
+  <x:si>
     <x:t>[Parte1] Assignment 1: Calculate Client Security Hash</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=dVscUkz5AMA</x:t>
   </x:si>
   <x:si>
+    <x:t>27 may 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>Video Demo - Fine-tuning Selectors with Variables || UiPath ...</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=5bYP_I75DG8</x:t>
   </x:si>
   <x:si>
-    <x:t>RPA Video Tutorials | UiPath | UI Automation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.uipath.com/learning/video-tutorials/topic/ui-automation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Working with UI elements || UiPath Academy - Video Demo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=ucFVNHOCzYY</x:t>
+    <x:t>RPA Video Tutorials | UiPath | Vlad Ionescu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.uipath.com/learning/video-tutorials/author/vlad-ionescu</x:t>
   </x:si>
   <x:si>
     <x:t>Video Demo - Editing a Selector using UI Explorer ... - YouTube</x:t>
@@ -457,12 +403,18 @@
     <x:t>https://m.youtube.com/watch?v=ASsqql9bBGU&amp;pp=ygUJI25vdGFzcnBh</x:t>
   </x:si>
   <x:si>
+    <x:t>Hace 1 mes</x:t>
+  </x:si>
+  <x:si>
     <x:t>[Ejecución]Dispatcher &amp; Performer| Orchestrator App Mobile ...</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=maQ_K7FcSAg</x:t>
   </x:si>
   <x:si>
+    <x:t>25 ago 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>RPA Video Tutorials | UiPath | Ioana Sabau</x:t>
   </x:si>
   <x:si>
@@ -475,12 +427,6 @@
     <x:t>https://www.youtube.com/watch?v=8XfPvDXZaoc</x:t>
   </x:si>
   <x:si>
-    <x:t>Cómo crear robots con UiPath - (Curso GRATIS en descripción)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.youtube.com/watch?v=JHjpwUe7tVc</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://www.youtube.com/watch?v=oTVDifE5SZo</x:t>
   </x:si>
   <x:si>
@@ -490,22 +436,325 @@
     <x:t>https://www.youtube.com/watch?v=ccYNle8sk-o</x:t>
   </x:si>
   <x:si>
+    <x:t>13 feb 2019</x:t>
+  </x:si>
+  <x:si>
     <x:t>How to Learn UiPath - Online Resources - YouTube</x:t>
   </x:si>
   <x:si>
     <x:t>https://m.youtube.com/watch?v=S8ydzPF_zqQ</x:t>
   </x:si>
   <x:si>
+    <x:t>22 ene 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Academy Live sessions at HIMSS22 - LinkedIn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://uk.linkedin.com/posts/uipath_uipath-academy-live-sessions-at-himss22-activity-6909854961329737728-Su1v?trk=public_profile_like_view</x:t>
+  </x:si>
+  <x:si>
     <x:t>Dispatcher &amp; REFramework Performer Demo || UiPath Academy</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=uSFCQ5usGxo</x:t>
   </x:si>
   <x:si>
+    <x:t>9 may 2020</x:t>
+  </x:si>
+  <x:si>
     <x:t>The Call Stack Panel - RPA Developer Foundation - YouTube</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.youtube.com/watch?v=VsW1lVUHDno</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Where to Start Learning RPA? - Beginners - @UiPath - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=JIopirJcbsY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 ene 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robots and Environments in Orchestrator || UiPath Academy ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=dNpQvPeeXYs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>If Statements || UiPath Academy || RPA Developer Foundation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://m.youtube.com/watch?v=RjGJidK2O-w</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 abr 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Breakpoints || UiPath Academy || RPA Developer Foundation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=2NbgyzcMdqU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Video Demo - Using Wildcards in Selectors || UiPath Academy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=QH530qJPNUI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=XzEYqeOEEWE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11 abr 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=ASsqql9bBGU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA Developer Foundation - Quiz 2: Data Manipulation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=twjSzwKvaDQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 may 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Debugging Interface || UiPath Academy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=nLJmydUBIB0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Free RPA Certifications with UiPath Academy Complete Guide</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=HUjLUa5CHJU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 may 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Task Automation with StudioX - UiPath</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.uipath.com/learning/video-tutorials/task-automation-with-studiox</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UIpath academy|Rpa citizen developer foundation answer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=w5k9CcOgOHc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 feb 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Studio / Studio X Installation Guide - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=DW8R2v5uPss</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 abr 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Essesntial Training - 4 3 Selectors</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.uipath.com/learning/video-tutorials/selectors</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA Tutorial | How-to Build Your First Bot in UiPath - Session 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=Z25nJygF9gg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23 dic 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Academy Generate Yearly Report Assignment - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=MnNG5I7xyHU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23 abr 2018</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reduce Blue Light and Change UiPath from White to Dark Mode</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=qXN7CBXBZIU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 may 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Studio X Tutorial: Become a Citizen RPA Developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=C1gWGaumBJA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 jul 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Academy - Solving RPA Advanced Part - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=WSJ03LSMBu0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 dic 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Uipath advanced training assignment 1 - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=12qLI2Z2Qz8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 mar 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Skillathon 2022 Masterclass 2 #UiPathSkillathon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=qcSxb5AKO04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20 ene 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA training in 30 days |better than academy - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=YixN6gmrnN4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21 ene 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath RPA Developer Certificate - Where to start? - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=PDecUWsgFv0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 mar 2019</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Tutorials | Episode - 09 | Knowledge of RPA - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=oDlnXMSdD0c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 feb 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=Lz19Kyc9pcE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20 dic 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Complete guide to prepare for UiPath Advanced RPA ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=FINGKncUOlE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 jul 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath | Alliances - Infosys</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.infosys.com/about/alliances/uipath.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://m.youtube.com/watch?v=HUjLUa5CHJU&amp;pp=ygUdI3VpcGF0aGRldmVsb3BlcmNlcnRpZmljYXRpb24%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30 ago 2023</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mason Turvey, Intelligent Automation Lead @Academy Bank ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=hfxG69cap6E</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Test Suite: Database Testing - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=a68Xjfbt5Hc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16 nov 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Calculate Client Security Hash - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=A-WBxyKijko</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 ago 2022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA Summer School Session 4: Automate Outlook and Gmail ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://community.uipath.com/events/details/uipath-citizen-developers-presents-rpa-summer-school-session-4-automate-outlook-and-gmail-with-ease-1/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Download Sample Invoice Receipts and Forms for UiPath ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=622F-xyNGD0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 jul 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Automation Use Cases || RPA Example with ... - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=UENa9FIsZFQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 may 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Curso de RPA con UiPath desde Cero en Español - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=ZtJp6ctP7TQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28 nov 2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UiPath Academy Live for Kids! - YouTube</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=eZI5jYjmvBk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crear robots Unattended sin Orchestrator | UiPath en Español</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.youtube.com/watch?v=Hka2zWhk_DY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19 may 2020</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -869,693 +1118,1076 @@
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="A8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:3">
+      <x:c r="A17" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="A25" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:3">
+      <x:c r="A26" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="A28" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:3">
+      <x:c r="A40" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>102</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>105</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:3">
+      <x:c r="A44" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:3">
       <x:c r="A46" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:3">
+      <x:c r="A47" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:3">
       <x:c r="A48" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:3">
       <x:c r="A49" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:3">
       <x:c r="A50" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>123</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:3">
+      <x:c r="A51" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:3">
       <x:c r="A52" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:3">
       <x:c r="A53" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>129</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:3">
       <x:c r="A54" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>132</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:3">
       <x:c r="A55" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:3">
       <x:c r="A56" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:3">
       <x:c r="A57" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:3">
       <x:c r="A58" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:3">
       <x:c r="A59" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:3">
       <x:c r="A60" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>145</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:3">
       <x:c r="A61" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:3">
       <x:c r="A62" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:3">
       <x:c r="A63" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:3">
       <x:c r="A64" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>148</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:3">
       <x:c r="A65" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:3">
       <x:c r="A66" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:3">
       <x:c r="A67" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="C67" s="0" t="s">
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:3">
       <x:c r="A68" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:3">
       <x:c r="A69" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:3">
+      <x:c r="A70" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>168</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:3">
       <x:c r="A71" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:3">
       <x:c r="A72" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:3">
       <x:c r="A73" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>175</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:3">
       <x:c r="A74" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>178</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:3">
       <x:c r="A75" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="C75" s="0" t="s">
+        <x:v>181</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:3">
       <x:c r="A76" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:3">
       <x:c r="A77" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>186</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:3">
       <x:c r="A78" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="C78" s="0" t="s">
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:3">
       <x:c r="A79" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>192</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:3">
       <x:c r="A80" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>194</x:v>
+      </x:c>
+      <x:c r="C80" s="0" t="s">
+        <x:v>195</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:3">
       <x:c r="A81" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:3">
       <x:c r="A82" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>201</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:3">
       <x:c r="A83" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>204</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:3">
       <x:c r="A84" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>206</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>207</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:3">
       <x:c r="A85" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>210</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:3">
       <x:c r="A86" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>212</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>213</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:3">
       <x:c r="A87" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:3">
       <x:c r="A88" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
+        <x:v>218</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:3">
       <x:c r="A89" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>220</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:3">
       <x:c r="A90" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>222</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:3">
       <x:c r="A91" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>224</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:3">
+      <x:c r="A92" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:3">
       <x:c r="A93" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>230</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:3">
       <x:c r="A94" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>232</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:3">
       <x:c r="A95" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:3">
+      <x:c r="A96" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>238</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:3">
       <x:c r="A97" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:3">
       <x:c r="A98" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>241</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:3">
+      <x:c r="A99" s="0" t="s">
+        <x:v>242</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:3">
       <x:c r="A100" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>245</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>246</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>